<commit_message>
Fix punctuation in saving reports
</commit_message>
<xml_diff>
--- a/front/src/assets/SOLICITAR_AHORRO_COMISION.xlsx
+++ b/front/src/assets/SOLICITAR_AHORRO_COMISION.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\femseapto\front\src\assets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF1C8F6-E04F-42E2-8076-D7A256444AA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Table 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Table 1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+  </extLst>
 </workbook>
 </file>
 
@@ -25,133 +21,9 @@
     <r>
       <rPr>
         <b/>
-        <sz val="8.5"/>
+        <sz val="18.5"/>
+        <color theme="1" tint="0.049989318521683403"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Seleccione la línea de ahorro que desea solicitar:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>ESPACIO EXCLUSIVO PARA FEMSEAPTO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Nota:</t>
-    </r>
-  </si>
-  <si>
-    <t>PÁGINA: 1 de 1</t>
-  </si>
-  <si>
-    <t>FIRMA: ______________________________________________________</t>
-  </si>
-  <si>
-    <t>NOMBRE: ____________________________________________________</t>
-  </si>
-  <si>
-    <t>CEDULA: _____________________________________________________</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Firma de recibido</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Firma de Creación</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Fecha de recibido</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Fecha de Creación</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Extraordinario</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8.5"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>: $__________________</t>
-    </r>
-  </si>
-  <si>
-    <t>Se debe anexar el estudio de capacidad de endeudamiento para cada solicitud de creación de ahorro y así validar si cuenta con la capacidad.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="18.5"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve">SOLICITUD DE AHORRO
 </t>
@@ -160,15 +32,20 @@
       <rPr>
         <b/>
         <sz val="14"/>
-        <color theme="1" tint="4.9989318521683403E-2"/>
+        <color theme="1" tint="0.049989318521683403"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
-      <t>ASOCIADOS COMISIÓN</t>
+      <t xml:space="preserve">ASOCIADOS COMISIÓN</t>
     </r>
   </si>
   <si>
-    <t>CODIGO: FR-GA-03</t>
+    <t xml:space="preserve">CODIGO: FR-GA-03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VERSIÓN: 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PÁGINA: 1 de 1</t>
   </si>
   <si>
     <r>
@@ -176,243 +53,229 @@
     </r>
     <r>
       <rPr>
-        <u/>
-        <sz val="8.5"/>
+        <u val="single"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t>                                                                                                              ___        </t>
     </r>
     <r>
       <rPr>
-        <sz val="8.5"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> Identificado     con     cédula N°</t>
     </r>
     <r>
       <rPr>
-        <u/>
-        <sz val="8.5"/>
+        <u val="single"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t>                                                                  </t>
     </r>
     <r>
       <rPr>
-        <sz val="8.5"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> de   </t>
     </r>
     <r>
       <rPr>
-        <u/>
-        <sz val="8.5"/>
+        <u val="single"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t>                                        </t>
     </r>
     <r>
       <rPr>
-        <sz val="8.5"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve">,   autorizo   a </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <u/>
-        <sz val="8.5"/>
+        <u val="single"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t>                                        </t>
     </r>
     <r>
       <rPr>
         <b/>
-        <sz val="8.5"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve">   </t>
     </r>
     <r>
       <rPr>
-        <sz val="8.5"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
-      <t>para   descontar   de   mi   salario   el   valor   de   $</t>
+      <t xml:space="preserve">para   descontar   de   mi   salario   el   valor   de   $</t>
     </r>
     <r>
       <rPr>
-        <u/>
-        <sz val="8.5"/>
+        <u val="single"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t>                    __  _             </t>
     </r>
     <r>
       <rPr>
-        <sz val="8.5"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> quincenalmente,  a partir de  la </t>
     </r>
     <r>
       <rPr>
-        <u/>
-        <sz val="8.5"/>
+        <u val="single"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t>                    ____               </t>
     </r>
     <r>
       <rPr>
-        <sz val="8.5"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t xml:space="preserve"> quincena de </t>
     </r>
     <r>
       <rPr>
-        <u/>
-        <sz val="8.5"/>
+        <u val="single"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t>                 __                            </t>
     </r>
     <r>
       <rPr>
-        <sz val="8.5"/>
+        <sz val="10"/>
         <rFont val="Calibri"/>
-        <family val="1"/>
       </rPr>
       <t>.</t>
     </r>
   </si>
   <si>
-    <t>CELULAR: ____________________________________________________</t>
+    <t xml:space="preserve">Seleccione la línea de ahorro que desea solicitar:</t>
   </si>
   <si>
-    <t>VERSIÓN: 2</t>
+    <t xml:space="preserve">Extraordinario: $__________________</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FIRMA: ______________________________________________________</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOMBRE: ____________________________________________________</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CEDULA: _____________________________________________________</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CELULAR: ____________________________________________________</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8.5"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t xml:space="preserve">ESPACIO EXCLUSIVO PARA FEMSEAPTO</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Firma de recibido:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de recibido:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Firma de Creación:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha de Creación:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8.5"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Nota:</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Se debe anexar el estudio de capacidad de endeudamiento para cada solicitud de creación de ahorro y así validar si cuenta con la capacidad.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="10">
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
+      <sz val="10.000000"/>
+      <color indexed="64"/>
       <name val="Times New Roman"/>
-      <charset val="204"/>
     </font>
     <font>
-      <sz val="8.5"/>
+      <sz val="11.000000"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="8.5"/>
+      <sz val="10.000000"/>
+      <color theme="1" tint="0.049989318521683403"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="8.5"/>
-      <name val="Calibri"/>
-      <family val="1"/>
+      <sz val="10.000000"/>
+      <color theme="1" tint="0.049989318521683403"/>
+      <name val="Times New Roman"/>
     </font>
     <font>
       <b/>
-      <sz val="8.5"/>
+      <sz val="10.000000"/>
+      <color indexed="64"/>
       <name val="Calibri"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="8.5"/>
-      <name val="Calibri"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="8.5"/>
-      <name val="Calibri"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18.5"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
-      <name val="Calibri"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="8.5"/>
+      <sz val="10.000000"/>
       <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8.5"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1" tint="4.9989318521683403E-2"/>
+      <sz val="10.000000"/>
       <name val="Calibri"/>
-      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8.500000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="8.500000"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="4">
@@ -424,76 +287,245 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB8CCE3"/>
+        <fgColor theme="0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFB8CCE3"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="29">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="none"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
@@ -508,201 +540,20 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -710,300 +561,314 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="none"/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="none"/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="none"/>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="73">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="68">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="2" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="2" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="3" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="2" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="4" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="4" fillId="0" borderId="5" numFmtId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="6" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="7" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="6" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="8" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="7" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="9" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="10" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="9" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="3" fillId="0" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="5" fillId="0" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="6" fillId="2" borderId="12" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="13" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="14" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="6" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="6" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="6" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="16" numFmtId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="17" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="18" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="6" fillId="2" borderId="19" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="6" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf fontId="7" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="20" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="21" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="15" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf fontId="7" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="3" borderId="4" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="3" borderId="22" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="3" borderId="5" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf fontId="6" fillId="2" borderId="23" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="6" fillId="2" borderId="24" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="24" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf fontId="6" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3" wrapText="1"/>
+    </xf>
+    <xf fontId="9" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="9" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="0" fillId="2" borderId="16" numFmtId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="6" fillId="2" borderId="25" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="3"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf fontId="6" fillId="2" borderId="26" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="9" fillId="2" borderId="27" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="9" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf fontId="9" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" indent="3" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="2" borderId="28" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="9" fillId="2" borderId="11" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="9" fillId="2" borderId="10" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1" vertical="center" wrapText="1"/>
+    </xf>
+    <xf fontId="8" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" indent="1" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Excel Built-in Normal" xfId="1" xr:uid="{AD9EDFFC-A056-424E-8728-DA962DF91EB8}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1016,7 +881,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:w="http://schemas.openxmlformats.org/wordprocessingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1027,30 +892,16 @@
     <xdr:ext cx="654376" cy="511869"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="image1.jpeg">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="5" name="image1.jpeg"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip r:embed="rId1"/>
+        <a:stretch/>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="565687" y="172962"/>
           <a:ext cx="654376" cy="511869"/>
@@ -1069,19 +920,13 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="436245" cy="393700"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:ext cx="436245" cy="393699"/>
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="10" name="Shape 4" descr="DD">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D20EBD7-5AB6-42CE-B620-2793E593AD66}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="10" name="Shape 4" descr="DD"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="4695825" y="3276600"/>
           <a:ext cx="436245" cy="393700"/>
@@ -1093,7 +938,7 @@
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="377951" y="0"/>
               </a:moveTo>
@@ -1207,7 +1052,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="57912" y="377951"/>
               </a:moveTo>
@@ -1222,7 +1067,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="377951" y="377951"/>
               </a:moveTo>
@@ -1237,7 +1082,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="387095" y="374903"/>
               </a:moveTo>
@@ -1258,7 +1103,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="48767" y="374903"/>
               </a:moveTo>
@@ -1273,7 +1118,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="405383" y="362711"/>
               </a:moveTo>
@@ -1300,7 +1145,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="30479" y="362711"/>
               </a:moveTo>
@@ -1315,7 +1160,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="417575" y="344423"/>
               </a:moveTo>
@@ -1345,7 +1190,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="24383" y="353567"/>
               </a:moveTo>
@@ -1360,7 +1205,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="18287" y="344423"/>
               </a:moveTo>
@@ -1375,7 +1220,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="430529" y="45719"/>
               </a:moveTo>
@@ -1411,7 +1256,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="19812" y="45719"/>
               </a:moveTo>
@@ -1426,7 +1271,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="420623" y="27431"/>
               </a:moveTo>
@@ -1456,7 +1301,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="25907" y="36575"/>
               </a:moveTo>
@@ -1471,7 +1316,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="33527" y="27431"/>
               </a:moveTo>
@@ -1486,7 +1331,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="406400" y="15239"/>
               </a:moveTo>
@@ -1513,7 +1358,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="54863" y="15239"/>
               </a:moveTo>
@@ -1528,7 +1373,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="402336" y="12191"/>
               </a:moveTo>
@@ -1566,13 +1411,20 @@
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="es-ES"/>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="es-ES"/>
             <a:t>    DD</a:t>
           </a:r>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1585,19 +1437,13 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>78867</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="433070" cy="393700"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:ext cx="433070" cy="393699"/>
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="Shape 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93101A62-AF40-4075-8E34-8EF389D1FC50}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="11" name="Shape 7"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="5223129" y="3279267"/>
           <a:ext cx="433070" cy="393700"/>
@@ -1609,7 +1455,7 @@
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="377951" y="0"/>
               </a:moveTo>
@@ -1699,7 +1545,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="387096" y="374903"/>
               </a:moveTo>
@@ -1720,7 +1566,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="45720" y="374903"/>
               </a:moveTo>
@@ -1735,7 +1581,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="405383" y="362712"/>
               </a:moveTo>
@@ -1762,7 +1608,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="414527" y="344424"/>
               </a:moveTo>
@@ -1789,7 +1635,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="16763" y="344424"/>
               </a:moveTo>
@@ -1804,7 +1650,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="428243" y="45719"/>
               </a:moveTo>
@@ -1834,7 +1680,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="18287" y="45719"/>
               </a:moveTo>
@@ -1849,7 +1695,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="417575" y="27431"/>
               </a:moveTo>
@@ -1876,7 +1722,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="405384" y="15239"/>
               </a:moveTo>
@@ -1903,7 +1749,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="51815" y="15239"/>
               </a:moveTo>
@@ -1918,7 +1764,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="402336" y="12191"/>
               </a:moveTo>
@@ -1956,13 +1802,20 @@
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="es-ES"/>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="es-ES"/>
             <a:t>   MM</a:t>
           </a:r>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1975,19 +1828,13 @@
       <xdr:row>14</xdr:row>
       <xdr:rowOff>78867</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="433070" cy="393700"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:ext cx="433070" cy="393699"/>
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="Shape 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{093C82A1-F161-4096-8B24-72D71CC364A8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="12" name="Shape 7"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="5737479" y="3279267"/>
           <a:ext cx="433070" cy="393700"/>
@@ -1999,7 +1846,7 @@
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="377951" y="0"/>
               </a:moveTo>
@@ -2089,7 +1936,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="387096" y="374903"/>
               </a:moveTo>
@@ -2110,7 +1957,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="45720" y="374903"/>
               </a:moveTo>
@@ -2125,7 +1972,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="405383" y="362712"/>
               </a:moveTo>
@@ -2152,7 +1999,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="414527" y="344424"/>
               </a:moveTo>
@@ -2179,7 +2026,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="16763" y="344424"/>
               </a:moveTo>
@@ -2194,7 +2041,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="428243" y="45719"/>
               </a:moveTo>
@@ -2224,7 +2071,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="18287" y="45719"/>
               </a:moveTo>
@@ -2239,7 +2086,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="417575" y="27431"/>
               </a:moveTo>
@@ -2266,7 +2113,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="405384" y="15239"/>
               </a:moveTo>
@@ -2293,7 +2140,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="51815" y="15239"/>
               </a:moveTo>
@@ -2308,7 +2155,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="402336" y="12191"/>
               </a:moveTo>
@@ -2346,13 +2193,20 @@
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="es-ES"/>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="es-ES"/>
             <a:t>    AA</a:t>
           </a:r>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2365,19 +2219,13 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="436245" cy="393700"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:ext cx="436245" cy="393699"/>
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="Shape 4" descr="DD">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4970496E-8AC8-45A6-B20C-7CE73E4C50D0}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="13" name="Shape 4" descr="DD"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="4695825" y="4181475"/>
           <a:ext cx="436245" cy="393700"/>
@@ -2389,7 +2237,7 @@
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="377951" y="0"/>
               </a:moveTo>
@@ -2503,7 +2351,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="57912" y="377951"/>
               </a:moveTo>
@@ -2518,7 +2366,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="377951" y="377951"/>
               </a:moveTo>
@@ -2533,7 +2381,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="387095" y="374903"/>
               </a:moveTo>
@@ -2554,7 +2402,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="48767" y="374903"/>
               </a:moveTo>
@@ -2569,7 +2417,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="405383" y="362711"/>
               </a:moveTo>
@@ -2596,7 +2444,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="30479" y="362711"/>
               </a:moveTo>
@@ -2611,7 +2459,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="417575" y="344423"/>
               </a:moveTo>
@@ -2641,7 +2489,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="24383" y="353567"/>
               </a:moveTo>
@@ -2656,7 +2504,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="18287" y="344423"/>
               </a:moveTo>
@@ -2671,7 +2519,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="430529" y="45719"/>
               </a:moveTo>
@@ -2707,7 +2555,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="19812" y="45719"/>
               </a:moveTo>
@@ -2722,7 +2570,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="420623" y="27431"/>
               </a:moveTo>
@@ -2752,7 +2600,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="25907" y="36575"/>
               </a:moveTo>
@@ -2767,7 +2615,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="33527" y="27431"/>
               </a:moveTo>
@@ -2782,7 +2630,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="406400" y="15239"/>
               </a:moveTo>
@@ -2809,7 +2657,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="54863" y="15239"/>
               </a:moveTo>
@@ -2824,7 +2672,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="436245" h="393700">
+            <a:path w="436245" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="402336" y="12191"/>
               </a:moveTo>
@@ -2862,13 +2710,20 @@
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="es-ES"/>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="es-ES"/>
             <a:t>    DD</a:t>
           </a:r>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2881,19 +2736,13 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>97917</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="433070" cy="393700"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:ext cx="433070" cy="393699"/>
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="14" name="Shape 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E31479F0-BCC4-4765-99BA-917E4DE3FBDD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="14" name="Shape 7"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="5223129" y="4184142"/>
           <a:ext cx="433070" cy="393700"/>
@@ -2905,7 +2754,7 @@
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="377951" y="0"/>
               </a:moveTo>
@@ -2995,7 +2844,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="387096" y="374903"/>
               </a:moveTo>
@@ -3016,7 +2865,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="45720" y="374903"/>
               </a:moveTo>
@@ -3031,7 +2880,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="405383" y="362712"/>
               </a:moveTo>
@@ -3058,7 +2907,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="414527" y="344424"/>
               </a:moveTo>
@@ -3085,7 +2934,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="16763" y="344424"/>
               </a:moveTo>
@@ -3100,7 +2949,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="428243" y="45719"/>
               </a:moveTo>
@@ -3130,7 +2979,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="18287" y="45719"/>
               </a:moveTo>
@@ -3145,7 +2994,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="417575" y="27431"/>
               </a:moveTo>
@@ -3172,7 +3021,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="405384" y="15239"/>
               </a:moveTo>
@@ -3199,7 +3048,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="51815" y="15239"/>
               </a:moveTo>
@@ -3214,7 +3063,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="402336" y="12191"/>
               </a:moveTo>
@@ -3252,13 +3101,20 @@
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="es-ES"/>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="es-ES"/>
             <a:t>   MM</a:t>
           </a:r>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3271,19 +3127,13 @@
       <xdr:row>15</xdr:row>
       <xdr:rowOff>97917</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="433070" cy="393700"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:ext cx="433070" cy="393699"/>
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="Shape 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38D0ACE9-D2D5-4C7D-BCB2-C30BBCE8F48F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="15" name="Shape 7"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="5737479" y="4184142"/>
           <a:ext cx="433070" cy="393700"/>
@@ -3295,7 +3145,7 @@
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="377951" y="0"/>
               </a:moveTo>
@@ -3385,7 +3235,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="387096" y="374903"/>
               </a:moveTo>
@@ -3406,7 +3256,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="45720" y="374903"/>
               </a:moveTo>
@@ -3421,7 +3271,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="405383" y="362712"/>
               </a:moveTo>
@@ -3448,7 +3298,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="414527" y="344424"/>
               </a:moveTo>
@@ -3475,7 +3325,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="16763" y="344424"/>
               </a:moveTo>
@@ -3490,7 +3340,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="428243" y="45719"/>
               </a:moveTo>
@@ -3520,7 +3370,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="18287" y="45719"/>
               </a:moveTo>
@@ -3535,7 +3385,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="417575" y="27431"/>
               </a:moveTo>
@@ -3562,7 +3412,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="405384" y="15239"/>
               </a:moveTo>
@@ -3589,7 +3439,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="51815" y="15239"/>
               </a:moveTo>
@@ -3604,7 +3454,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="433070" h="393700">
+            <a:path w="433070" h="393700" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="402336" y="12191"/>
               </a:moveTo>
@@ -3642,13 +3492,20 @@
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="es-ES"/>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="es-ES"/>
             <a:t>    AA</a:t>
           </a:r>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -3661,19 +3518,13 @@
       <xdr:row>8</xdr:row>
       <xdr:rowOff>69850</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="917576" cy="1045846"/>
-    <xdr:sp macro="" textlink="">
+    <xdr:ext cx="917576" cy="1045845"/>
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="Shape 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB0BF01D-2A2D-49B1-8DF1-752535ACE0E7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="16" name="Shape 3"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="4238625" y="1974850"/>
           <a:ext cx="917576" cy="1045846"/>
@@ -3685,7 +3536,7 @@
           <a:cxnLst/>
           <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
-            <a:path w="744220" h="744220">
+            <a:path w="744220" h="744220" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="124967" y="3048"/>
               </a:moveTo>
@@ -3820,7 +3671,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="744220" h="744220">
+            <a:path w="744220" h="744220" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="737615" y="88391"/>
               </a:moveTo>
@@ -3862,7 +3713,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="744220" h="744220">
+            <a:path w="744220" h="744220" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="10668" y="88391"/>
               </a:moveTo>
@@ -3877,7 +3728,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="744220" h="744220">
+            <a:path w="744220" h="744220" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="643127" y="3048"/>
               </a:moveTo>
@@ -3931,7 +3782,7 @@
               </a:lnTo>
               <a:close/>
             </a:path>
-            <a:path w="744220" h="744220">
+            <a:path w="744220" h="744220" fill="norm" stroke="1" extrusionOk="0">
               <a:moveTo>
                 <a:pt x="618744" y="0"/>
               </a:moveTo>
@@ -3968,20 +3819,33 @@
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="es-ES"/>
             <a:t>     </a:t>
           </a:r>
+          <a:endParaRPr/>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="es-ES"/>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:endParaRPr lang="es-ES"/>
         </a:p>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
-            <a:rPr lang="es-ES" baseline="0"/>
+            <a:rPr lang="es-ES"/>
             <a:t>     </a:t>
           </a:r>
           <a:endParaRPr lang="es-ES"/>
@@ -3990,7 +3854,7 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="twoCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
       <xdr:colOff>850900</xdr:colOff>
@@ -4001,23 +3865,17 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>1543050</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:rowOff>196849</xdr:rowOff>
     </xdr:to>
-    <xdr:sp macro="" textlink="">
+    <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="CuadroTexto 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A0A0DCA-F36A-2492-6608-69943BBC787F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="CuadroTexto 1"/>
         <xdr:cNvSpPr txBox="1"/>
       </xdr:nvSpPr>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="4438650" y="2838450"/>
-          <a:ext cx="692150" cy="215900"/>
+          <a:ext cx="692150" cy="215899"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4029,13 +3887,13 @@
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:lnRef>
         <a:fillRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:fillRef>
         <a:effectRef idx="0">
-          <a:scrgbClr r="0" g="0" b="0"/>
+          <a:srgbClr val="000000"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="dk1"/>
@@ -4045,10 +3903,14 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:pPr>
+            <a:defRPr/>
+          </a:pPr>
           <a:r>
             <a:rPr lang="es-CO" sz="800" b="1"/>
             <a:t>HUELLA</a:t>
           </a:r>
+          <a:endParaRPr/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -4063,30 +3925,22 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>47783</xdr:colOff>
+      <xdr:colOff>47782</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>161</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{987D48F4-ACA6-F8F5-7024-7EE77459CB3D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Imagen 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip r:embed="rId2"/>
+        <a:stretch/>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="3810000" y="1933575"/>
           <a:ext cx="1133633" cy="1152686"/>
@@ -4113,24 +3967,16 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{253ACB71-3E3B-8504-0BEC-2369EFE450B8}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Imagen 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
+        <a:blip r:embed="rId3"/>
+        <a:stretch/>
       </xdr:blipFill>
-      <xdr:spPr>
+      <xdr:spPr bwMode="auto">
         <a:xfrm>
           <a:off x="4610100" y="3476625"/>
           <a:ext cx="1667108" cy="962159"/>
@@ -4145,10 +3991,10 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2007 - 2010">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -4186,18 +4032,18 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2007 - 2010">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -4220,19 +4066,18 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Cordia New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -4255,10 +4100,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2007 - 2010">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4430,401 +4274,611 @@
 </a:theme>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme 2007 - 2010">
+  <a:themeElements>
+    <a:clrScheme name="Office 2007 - 2010">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office 2007 - 2010">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office 2007 - 2010">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle"/>
+        </a:gradFill>
+        <a:gradFill>
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J37"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
+      <selection activeCell="Q13" activeCellId="0" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="12"/>
   <cols>
-    <col min="1" max="1" width="4.83203125" style="16" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="5.33203125" customWidth="1"/>
-    <col min="5" max="5" width="23.5" customWidth="1"/>
-    <col min="6" max="6" width="29.1640625" customWidth="1"/>
-    <col min="7" max="7" width="8" customWidth="1"/>
-    <col min="8" max="8" width="11.1640625" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="4.83203125" style="16" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" style="1" width="4.83203125"/>
+    <col customWidth="1" min="2" max="2" width="10.1640625"/>
+    <col customWidth="1" min="3" max="3" width="12.6640625"/>
+    <col customWidth="1" min="4" max="4" width="5.33203125"/>
+    <col customWidth="1" min="5" max="5" width="23.5"/>
+    <col customWidth="1" min="6" max="6" width="29.1640625"/>
+    <col customWidth="1" min="7" max="7" width="8"/>
+    <col customWidth="1" min="8" max="8" width="11.1640625"/>
+    <col customWidth="1" min="9" max="9" width="12.1640625"/>
+    <col customWidth="1" min="10" max="10" style="1" width="4.83203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="11.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
+    <row r="1" ht="11.449999999999999" customHeight="1">
+      <c r="A1" s="2"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="38"/>
-      <c r="B2" s="67"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="58" t="s">
+    <row r="2" ht="15" customHeight="1">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="10"/>
+      <c r="J2" s="3"/>
+    </row>
+    <row r="3" ht="15" customHeight="1">
+      <c r="A3" s="3"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I3" s="10"/>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" ht="15" customHeight="1">
+      <c r="A4" s="3"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="22"/>
+      <c r="J4" s="3"/>
+    </row>
+    <row r="5" ht="45.75" customHeight="1">
+      <c r="A5" s="3"/>
+      <c r="B5" s="23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
+      <c r="H5" s="24"/>
+      <c r="I5" s="25"/>
+      <c r="J5" s="3"/>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="3"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="27"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="27"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="3"/>
+    </row>
+    <row r="7" ht="20.25" customHeight="1">
+      <c r="A7" s="3"/>
+      <c r="B7" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="32"/>
+      <c r="J7" s="3"/>
+    </row>
+    <row r="8" ht="12.75" customHeight="1">
+      <c r="A8" s="3"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="34"/>
+      <c r="D8" s="35"/>
+      <c r="E8" s="36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8" s="37"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="3"/>
+    </row>
+    <row r="9" ht="40.5" customHeight="1">
+      <c r="A9" s="3"/>
+      <c r="B9" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="40"/>
+      <c r="D9" s="40"/>
+      <c r="E9" s="40"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="3"/>
+    </row>
+    <row r="10" ht="17.25" customHeight="1">
+      <c r="A10" s="3"/>
+      <c r="B10" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40"/>
+      <c r="E10" s="40"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="3"/>
+    </row>
+    <row r="11" s="42" customFormat="1" ht="17.449999999999999" customHeight="1">
+      <c r="A11" s="3"/>
+      <c r="B11" s="39" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="3"/>
+    </row>
+    <row r="12" s="42" customFormat="1" ht="17.449999999999999" customHeight="1">
+      <c r="A12" s="3"/>
+      <c r="B12" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="44"/>
+      <c r="D12" s="44"/>
+      <c r="E12" s="44"/>
+      <c r="F12" s="44"/>
+      <c r="G12" s="44"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="3"/>
+    </row>
+    <row r="13" s="42" customFormat="1" ht="13.5" customHeight="1">
+      <c r="A13" s="3"/>
+      <c r="B13" s="46"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="48"/>
+      <c r="J13" s="3"/>
+    </row>
+    <row r="14" ht="12.75" customHeight="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="49" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="3"/>
+    </row>
+    <row r="15" ht="37.5" customHeight="1">
+      <c r="A15" s="3"/>
+      <c r="B15" s="52" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="53"/>
+      <c r="D15" s="54"/>
+      <c r="E15" s="54"/>
+      <c r="F15" s="55" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="59"/>
-      <c r="F2" s="59"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="24" t="s">
+      <c r="G15" s="56"/>
+      <c r="H15" s="57"/>
+      <c r="I15" s="58"/>
+      <c r="J15" s="3"/>
+    </row>
+    <row r="16" ht="37.5" customHeight="1">
+      <c r="A16" s="3"/>
+      <c r="B16" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="25"/>
-      <c r="J2" s="38"/>
+      <c r="C16" s="60"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="55" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="56"/>
+      <c r="H16" s="57"/>
+      <c r="I16" s="58"/>
+      <c r="J16" s="3"/>
     </row>
-    <row r="3" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="38"/>
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="24" t="s">
+    <row r="17" ht="10.5" customHeight="1">
+      <c r="A17" s="3"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="62"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="56"/>
+      <c r="H17" s="57"/>
+      <c r="I17" s="58"/>
+      <c r="J17" s="3"/>
+    </row>
+    <row r="18" ht="32.25" customHeight="1">
+      <c r="A18" s="3"/>
+      <c r="B18" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="25"/>
-      <c r="J3" s="38"/>
+      <c r="D18" s="65"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="65"/>
+      <c r="G18" s="65"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="66"/>
+      <c r="J18" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="38"/>
-      <c r="B4" s="71"/>
-      <c r="C4" s="72"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="65"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="22" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="38"/>
+    <row r="19" ht="32.25" customHeight="1">
+      <c r="A19" s="3"/>
+      <c r="B19" s="67"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="3"/>
     </row>
-    <row r="5" spans="1:10" ht="45.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="38"/>
-      <c r="B5" s="40" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="38"/>
+    <row r="20" ht="32.25" customHeight="1">
+      <c r="A20" s="3"/>
+      <c r="B20" s="67"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="3"/>
     </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="38"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="38"/>
+    <row r="21" ht="23.25" customHeight="1">
+      <c r="A21" s="31"/>
+      <c r="J21" s="31"/>
     </row>
-    <row r="7" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="38"/>
-      <c r="B7" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="47"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="38"/>
+    <row r="22" ht="18.949999999999999" customHeight="1">
+      <c r="A22" s="3"/>
+      <c r="J22" s="3"/>
     </row>
-    <row r="8" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="38"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="49"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="26" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="27"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="38"/>
+    <row r="23" ht="12.949999999999999" customHeight="1">
+      <c r="A23" s="3"/>
+      <c r="J23" s="3"/>
     </row>
-    <row r="9" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="38"/>
-      <c r="B9" s="50" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="34"/>
-      <c r="E9" s="34"/>
-      <c r="F9" s="34"/>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="35"/>
-      <c r="J9" s="38"/>
+    <row r="24" ht="16.699999999999999" customHeight="1">
+      <c r="A24" s="3"/>
+      <c r="J24" s="3"/>
     </row>
-    <row r="10" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="38"/>
-      <c r="B10" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="32"/>
-      <c r="D10" s="32"/>
-      <c r="E10" s="32"/>
-      <c r="F10" s="32"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="38"/>
+    <row r="25" ht="45.950000000000003" customHeight="1">
+      <c r="A25" s="3"/>
+      <c r="J25" s="3"/>
     </row>
-    <row r="11" spans="1:10" s="4" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="38"/>
-      <c r="B11" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-      <c r="G11" s="34"/>
-      <c r="H11" s="34"/>
-      <c r="I11" s="35"/>
-      <c r="J11" s="38"/>
+    <row r="26" ht="16.699999999999999" customHeight="1">
+      <c r="A26" s="3"/>
+      <c r="J26" s="3"/>
     </row>
-    <row r="12" spans="1:10" s="4" customFormat="1" ht="17.45" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="38"/>
-      <c r="B12" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="20"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="20"/>
-      <c r="I12" s="21"/>
-      <c r="J12" s="38"/>
+    <row r="27" ht="27.600000000000001" customHeight="1">
+      <c r="A27" s="3"/>
+      <c r="J27" s="3"/>
     </row>
-    <row r="13" spans="1:10" s="4" customFormat="1" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="28"/>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="29"/>
-      <c r="H13" s="29"/>
-      <c r="I13" s="30"/>
-      <c r="J13" s="38"/>
+    <row r="28" ht="12.75" customHeight="1">
+      <c r="A28" s="3"/>
+      <c r="J28" s="3"/>
     </row>
-    <row r="14" spans="1:10" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="38"/>
+    <row r="29" ht="40.5" customHeight="1">
+      <c r="A29" s="3"/>
+      <c r="J29" s="3"/>
     </row>
-    <row r="15" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="38"/>
-      <c r="B15" s="54" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="55"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="G15" s="12"/>
-      <c r="H15" s="9"/>
-      <c r="I15" s="10"/>
-      <c r="J15" s="38"/>
+    <row r="30" ht="17.25" customHeight="1">
+      <c r="A30" s="3"/>
+      <c r="J30" s="3"/>
     </row>
-    <row r="16" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="38"/>
-      <c r="B16" s="56" t="s">
-        <v>8</v>
-      </c>
-      <c r="C16" s="57"/>
-      <c r="D16" s="57"/>
-      <c r="E16" s="57"/>
-      <c r="F16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="38"/>
+    <row r="31" ht="17.25" customHeight="1">
+      <c r="A31" s="3"/>
+      <c r="J31" s="3"/>
     </row>
-    <row r="17" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="38"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="38"/>
+    <row r="32" ht="13.5" customHeight="1">
+      <c r="A32" s="3"/>
+      <c r="J32" s="3"/>
     </row>
-    <row r="18" spans="1:10" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="38"/>
-      <c r="B18" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="36"/>
-      <c r="F18" s="36"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="36"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="38"/>
+    <row r="33" ht="12.75" customHeight="1">
+      <c r="A33" s="3"/>
+      <c r="J33" s="3"/>
     </row>
-    <row r="19" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="17"/>
+    <row r="34" ht="37.5" customHeight="1">
+      <c r="A34" s="3"/>
+      <c r="J34" s="3"/>
     </row>
-    <row r="20" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="18"/>
-      <c r="C20" s="19"/>
-      <c r="D20" s="19"/>
-      <c r="E20" s="19"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="19"/>
-      <c r="H20" s="19"/>
-      <c r="I20" s="19"/>
-      <c r="J20" s="17"/>
+    <row r="35" ht="37.5" customHeight="1">
+      <c r="A35" s="3"/>
+      <c r="J35" s="3"/>
     </row>
-    <row r="21" spans="1:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
-      <c r="J21" s="3"/>
+    <row r="36" ht="10.5" customHeight="1">
+      <c r="A36" s="3"/>
+      <c r="J36" s="3"/>
     </row>
-    <row r="22" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="38"/>
-      <c r="J22" s="38"/>
-    </row>
-    <row r="23" spans="1:10" ht="12.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="38"/>
-      <c r="J23" s="38"/>
-    </row>
-    <row r="24" spans="1:10" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="38"/>
-      <c r="J24" s="38"/>
-    </row>
-    <row r="25" spans="1:10" ht="45.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="38"/>
-      <c r="J25" s="38"/>
-    </row>
-    <row r="26" spans="1:10" ht="16.7" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="38"/>
-      <c r="J26" s="38"/>
-    </row>
-    <row r="27" spans="1:10" ht="27.6" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="38"/>
-      <c r="J27" s="38"/>
-    </row>
-    <row r="28" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="38"/>
-      <c r="J28" s="38"/>
-    </row>
-    <row r="29" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="38"/>
-      <c r="J29" s="38"/>
-    </row>
-    <row r="30" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="38"/>
-      <c r="J30" s="38"/>
-    </row>
-    <row r="31" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="38"/>
-      <c r="J31" s="38"/>
-    </row>
-    <row r="32" spans="1:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="38"/>
-      <c r="J32" s="38"/>
-    </row>
-    <row r="33" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="38"/>
-      <c r="J33" s="38"/>
-    </row>
-    <row r="34" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="38"/>
-      <c r="J34" s="38"/>
-    </row>
-    <row r="35" spans="1:10" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="38"/>
-      <c r="J35" s="38"/>
-    </row>
-    <row r="36" spans="1:10" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="38"/>
-      <c r="J36" s="38"/>
-    </row>
-    <row r="37" spans="1:10" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" ht="32.25" customHeight="1">
       <c r="A37" s="2"/>
       <c r="J37" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="C18:I18"/>
-    <mergeCell ref="A22:A36"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:A18"/>
+    <mergeCell ref="B2:C4"/>
+    <mergeCell ref="D2:G4"/>
+    <mergeCell ref="H2:I2"/>
     <mergeCell ref="J2:J18"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="H4:I4"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="B6:I6"/>
     <mergeCell ref="B7:E7"/>
     <mergeCell ref="B8:C8"/>
+    <mergeCell ref="E8:F8"/>
     <mergeCell ref="B9:I9"/>
+    <mergeCell ref="B10:I10"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="B16:E16"/>
+    <mergeCell ref="C18:I18"/>
+    <mergeCell ref="A22:A36"/>
     <mergeCell ref="J22:J36"/>
-    <mergeCell ref="D2:G4"/>
-    <mergeCell ref="B2:C4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="H3:I3"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B12:E12"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <printOptions headings="0" gridLines="0"/>
+  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
+  <pageSetup paperSize="9" scale="80" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>